<commit_message>
Finalização da funcionalidade de criar usuários alunos através da importação de um arquivo .xlsx
</commit_message>
<xml_diff>
--- a/Backend/static/modelo_criacao_usuario_aluno.xlsx
+++ b/Backend/static/modelo_criacao_usuario_aluno.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Modelo de importação para a Criação de usuário Aluno</t>
   </si>
@@ -25,6 +25,15 @@
   </si>
   <si>
     <t xml:space="preserve">Matricula do Aluno</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>Felipe</t>
+  </si>
+  <si>
+    <t>Rute</t>
   </si>
 </sst>
 </file>
@@ -80,7 +89,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -95,6 +104,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -635,191 +647,203 @@
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5">
+        <v>123524163</v>
+      </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5">
+        <v>147548120</v>
+      </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5">
+        <v>954715956</v>
+      </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="5"/>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="4"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="5"/>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="4"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="5"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="5"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="4"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="5"/>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="4"/>
+      <c r="A12" s="6"/>
       <c r="B12" s="5"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="4"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="5"/>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="4"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="5"/>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="4"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="5"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="4"/>
+      <c r="A16" s="6"/>
       <c r="B16" s="5"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="4"/>
+      <c r="A17" s="6"/>
       <c r="B17" s="5"/>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="5"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="4"/>
+      <c r="A19" s="6"/>
       <c r="B19" s="5"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="6"/>
       <c r="B20" s="5"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="4"/>
+      <c r="A21" s="6"/>
       <c r="B21" s="5"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="4"/>
+      <c r="A22" s="6"/>
       <c r="B22" s="5"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="4"/>
+      <c r="A23" s="6"/>
       <c r="B23" s="5"/>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="4"/>
+      <c r="A24" s="6"/>
       <c r="B24" s="5"/>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="4"/>
+      <c r="A25" s="6"/>
       <c r="B25" s="5"/>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="4"/>
+      <c r="A26" s="6"/>
       <c r="B26" s="5"/>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="4"/>
+      <c r="A27" s="6"/>
       <c r="B27" s="5"/>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="4"/>
+      <c r="A28" s="6"/>
       <c r="B28" s="5"/>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="4"/>
+      <c r="A29" s="6"/>
       <c r="B29" s="5"/>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="4"/>
+      <c r="A30" s="6"/>
       <c r="B30" s="5"/>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" s="4"/>
+      <c r="A31" s="6"/>
       <c r="B31" s="5"/>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" s="4"/>
+      <c r="A32" s="6"/>
       <c r="B32" s="5"/>
     </row>
     <row r="33" ht="14.25">
-      <c r="A33" s="4"/>
+      <c r="A33" s="6"/>
       <c r="B33" s="5"/>
     </row>
     <row r="34" ht="14.25">
-      <c r="A34" s="4"/>
+      <c r="A34" s="6"/>
       <c r="B34" s="5"/>
     </row>
     <row r="35" ht="14.25">
-      <c r="A35" s="4"/>
+      <c r="A35" s="6"/>
       <c r="B35" s="5"/>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="4"/>
+      <c r="A36" s="6"/>
       <c r="B36" s="5"/>
     </row>
     <row r="37" ht="14.25">
-      <c r="A37" s="4"/>
+      <c r="A37" s="6"/>
       <c r="B37" s="5"/>
     </row>
     <row r="38" ht="14.25">
-      <c r="A38" s="4"/>
+      <c r="A38" s="6"/>
       <c r="B38" s="5"/>
     </row>
     <row r="39" ht="14.25">
-      <c r="A39" s="4"/>
+      <c r="A39" s="6"/>
       <c r="B39" s="5"/>
     </row>
     <row r="40" ht="14.25">
-      <c r="A40" s="4"/>
+      <c r="A40" s="6"/>
       <c r="B40" s="5"/>
     </row>
     <row r="41" ht="14.25">
-      <c r="A41" s="4"/>
+      <c r="A41" s="6"/>
       <c r="B41" s="5"/>
     </row>
     <row r="42" ht="14.25">
-      <c r="A42" s="4"/>
+      <c r="A42" s="6"/>
       <c r="B42" s="5"/>
     </row>
     <row r="43" ht="14.25">
-      <c r="A43" s="4"/>
+      <c r="A43" s="6"/>
       <c r="B43" s="5"/>
     </row>
     <row r="44" ht="14.25">
-      <c r="A44" s="4"/>
+      <c r="A44" s="6"/>
       <c r="B44" s="5"/>
     </row>
     <row r="45" ht="14.25">
-      <c r="A45" s="4"/>
+      <c r="A45" s="6"/>
       <c r="B45" s="5"/>
     </row>
     <row r="46" ht="14.25">
-      <c r="A46" s="4"/>
+      <c r="A46" s="6"/>
       <c r="B46" s="5"/>
     </row>
     <row r="47" ht="14.25">
-      <c r="A47" s="4"/>
+      <c r="A47" s="6"/>
       <c r="B47" s="5"/>
     </row>
     <row r="48" ht="14.25">
-      <c r="A48" s="4"/>
+      <c r="A48" s="6"/>
       <c r="B48" s="5"/>
     </row>
     <row r="49" ht="14.25">
-      <c r="A49" s="4"/>
+      <c r="A49" s="6"/>
       <c r="B49" s="5"/>
     </row>
     <row r="50" ht="14.25">
-      <c r="A50" s="4"/>
+      <c r="A50" s="6"/>
       <c r="B50" s="5"/>
     </row>
   </sheetData>

</xml_diff>